<commit_message>
Don't add zero stack adjuments when functions don't use stack
</commit_message>
<xml_diff>
--- a/contrib/bwilks/benchmarking/New Graphs.xlsx
+++ b/contrib/bwilks/benchmarking/New Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\helix\contrib\bwilks\benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563867F3-4425-46A0-B6C4-A6941F17D3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238848CD-171A-40B4-9632-DF27D6E056DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="3600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.34</c:v>
+                  <c:v>6.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>84.7</c:v>
@@ -2288,7 +2288,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7.34</c:v>
+                  <c:v>6.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>84.7</c:v>
@@ -7218,8 +7218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,7 +7263,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>7.34</v>
+        <v>6.67</v>
       </c>
       <c r="E5">
         <v>84.7</v>

</xml_diff>